<commit_message>
Created more models with more flexibility in the S1 and S2 parameters
</commit_message>
<xml_diff>
--- a/models/Richards Model Parameters.xlsx
+++ b/models/Richards Model Parameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomo.eguchi\Documents\R\Granite_Canyon_Counts\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A1A81A-1BE5-4DA1-BBE8-E4EAD070A2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6259F1-951B-4E8B-832B-1A7B5857BA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="1710" windowWidth="19110" windowHeight="19620" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
+    <workbookView xWindow="2355" yWindow="540" windowWidth="19110" windowHeight="19620" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="20">
   <si>
     <t>K1</t>
   </si>
@@ -90,7 +91,10 @@
     <t>Model numbers in manuscript</t>
   </si>
   <si>
-    <t>Version numbers</t>
+    <t>Version numbers on model files</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -144,11 +148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,25 +470,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8830AAF-8B49-4DC6-B64F-BE0D27E1F80D}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="161.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -573,52 +583,55 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -628,202 +641,199 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7">
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>6</v>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I11" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>6</v>
-      </c>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="3">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="s">
-        <v>6</v>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -833,182 +843,173 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" t="s">
-        <v>6</v>
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="3">
-        <v>11</v>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>8</v>
@@ -1021,60 +1022,69 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="A22">
         <v>7</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" t="s">
-        <v>6</v>
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" t="s">
-        <v>6</v>
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>11</v>
-      </c>
       <c r="B24" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
@@ -1089,21 +1099,18 @@
         <v>6</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I24" s="3">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>12</v>
-      </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>9</v>
@@ -1118,18 +1125,18 @@
         <v>8</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I25" s="3">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1144,6 +1151,321 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Negative binomial models created
</commit_message>
<xml_diff>
--- a/models/Richards Model Parameters.xlsx
+++ b/models/Richards Model Parameters.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomo.eguchi\Documents\R\Granite_Canyon_Counts\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6259F1-951B-4E8B-832B-1A7B5857BA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415586F9-BBE1-45E6-8CCA-41F97B51626F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="540" windowWidth="19110" windowHeight="19620" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
+    <workbookView xWindow="3900" yWindow="1980" windowWidth="19110" windowHeight="19620" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -473,7 +475,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +585,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -609,6 +614,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -711,7 +719,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
@@ -740,7 +748,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -768,6 +776,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
@@ -794,6 +805,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
@@ -844,7 +858,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -873,7 +887,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>10</v>
@@ -901,6 +915,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
@@ -927,6 +944,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +1043,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>10</v>
@@ -1052,7 +1072,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
@@ -1080,6 +1100,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>15</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
@@ -1106,6 +1129,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>16</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>10</v>
       </c>
@@ -1159,7 +1185,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
@@ -1188,7 +1214,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
@@ -1216,6 +1242,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>19</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
@@ -1242,6 +1271,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
@@ -1338,7 +1370,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>6</v>
@@ -1367,7 +1399,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>6</v>
@@ -1395,6 +1427,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>23</v>
+      </c>
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
@@ -1421,6 +1456,9 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>24</v>
+      </c>
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Model comparison script and updated manuscript
</commit_message>
<xml_diff>
--- a/models/Richards Model Parameters.xlsx
+++ b/models/Richards Model Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomo.eguchi\Documents\R\Granite_Canyon_Counts\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415586F9-BBE1-45E6-8CCA-41F97B51626F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB28DE0-1C61-4737-9304-D744AC38E701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1980" windowWidth="19110" windowHeight="19620" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
+    <workbookView xWindow="1740" yWindow="2745" windowWidth="19110" windowHeight="18000" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="53">
   <si>
     <t>K1</t>
   </si>
@@ -97,6 +97,105 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>LOOIC</t>
+  </si>
+  <si>
+    <t>Nhats</t>
+  </si>
+  <si>
+    <t>Horrible</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>n.big.Rhat</t>
+  </si>
+  <si>
+    <t>n.bad.Pareto</t>
+  </si>
+  <si>
+    <t>p.bad.Pareto</t>
+  </si>
+  <si>
+    <t>v2a</t>
+  </si>
+  <si>
+    <t>v15a</t>
+  </si>
+  <si>
+    <t>v17a</t>
+  </si>
+  <si>
+    <t>v18a</t>
+  </si>
+  <si>
+    <t>v5a</t>
+  </si>
+  <si>
+    <t>v16a</t>
+  </si>
+  <si>
+    <t>v19a</t>
+  </si>
+  <si>
+    <t>v20a</t>
+  </si>
+  <si>
+    <t>v1a</t>
+  </si>
+  <si>
+    <t>v13a</t>
+  </si>
+  <si>
+    <t>v21a</t>
+  </si>
+  <si>
+    <t>v22a</t>
+  </si>
+  <si>
+    <t>v3a</t>
+  </si>
+  <si>
+    <t>v12a</t>
+  </si>
+  <si>
+    <t>v23a</t>
+  </si>
+  <si>
+    <t>v24a</t>
+  </si>
+  <si>
+    <t>v10a</t>
+  </si>
+  <si>
+    <t>v11a</t>
+  </si>
+  <si>
+    <t>v25a</t>
+  </si>
+  <si>
+    <t>v26a</t>
+  </si>
+  <si>
+    <t>v9a</t>
+  </si>
+  <si>
+    <t>v14a</t>
+  </si>
+  <si>
+    <t>v27a</t>
+  </si>
+  <si>
+    <t>v28a</t>
+  </si>
+  <si>
+    <t>Okay</t>
   </si>
 </sst>
 </file>
@@ -112,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +236,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -150,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -158,6 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,15 +578,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8830AAF-8B49-4DC6-B64F-BE0D27E1F80D}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="161.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="161.25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -496,8 +602,26 @@
       <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -525,8 +649,9 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -554,8 +679,23 @@
       <c r="I3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3">
+        <v>18456.255457203501</v>
+      </c>
+      <c r="L3">
+        <v>228</v>
+      </c>
+      <c r="M3">
+        <v>73</v>
+      </c>
+      <c r="N3">
+        <v>3.19195452557936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -583,8 +723,23 @@
       <c r="I4" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4">
+        <v>19096.250028757098</v>
+      </c>
+      <c r="L4">
+        <v>98</v>
+      </c>
+      <c r="M4">
+        <v>96</v>
+      </c>
+      <c r="N4">
+        <v>4.1976388281591603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -612,8 +767,23 @@
       <c r="I5" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5">
+        <v>18560.823535380601</v>
+      </c>
+      <c r="L5">
+        <v>59</v>
+      </c>
+      <c r="M5">
+        <v>54</v>
+      </c>
+      <c r="N5">
+        <v>2.3611718408395301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -641,8 +811,23 @@
       <c r="I6" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <v>18567.872387375799</v>
+      </c>
+      <c r="L6">
+        <v>68</v>
+      </c>
+      <c r="M6">
+        <v>70</v>
+      </c>
+      <c r="N6">
+        <v>3.0607783121993899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -665,7 +850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -691,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -717,8 +902,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -745,9 +930,27 @@
       <c r="I10" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>18377.009181113299</v>
+      </c>
+      <c r="L10">
+        <v>53</v>
+      </c>
+      <c r="M10">
+        <v>51</v>
+      </c>
+      <c r="N10">
+        <v>2.2299956274595498</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -774,9 +977,27 @@
       <c r="I11" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11">
+        <v>19179.086074593601</v>
+      </c>
+      <c r="L11">
+        <v>33</v>
+      </c>
+      <c r="M11">
+        <v>82</v>
+      </c>
+      <c r="N11">
+        <v>3.5854831657192801</v>
+      </c>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -803,9 +1024,27 @@
       <c r="I12" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12">
+        <v>18567.4568986698</v>
+      </c>
+      <c r="L12">
+        <v>44</v>
+      </c>
+      <c r="M12">
+        <v>57</v>
+      </c>
+      <c r="N12">
+        <v>2.4923480542194998</v>
+      </c>
+      <c r="O12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -832,8 +1071,26 @@
       <c r="I13" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13">
+        <v>18620.3893099698</v>
+      </c>
+      <c r="L13">
+        <v>49</v>
+      </c>
+      <c r="M13">
+        <v>57</v>
+      </c>
+      <c r="N13">
+        <v>2.4923480542194998</v>
+      </c>
+      <c r="O13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -856,7 +1113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -884,8 +1141,23 @@
       <c r="I15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15">
+        <v>18476.116777521998</v>
+      </c>
+      <c r="L15">
+        <v>258</v>
+      </c>
+      <c r="M15">
+        <v>68</v>
+      </c>
+      <c r="N15">
+        <v>2.97332750327941</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -913,8 +1185,23 @@
       <c r="I16" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16">
+        <v>18602.501768599399</v>
+      </c>
+      <c r="L16">
+        <v>76</v>
+      </c>
+      <c r="M16">
+        <v>78</v>
+      </c>
+      <c r="N16">
+        <v>3.4105815478793202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -942,8 +1229,23 @@
       <c r="I17" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17">
+        <v>18370.9522984711</v>
+      </c>
+      <c r="L17">
+        <v>166</v>
+      </c>
+      <c r="M17">
+        <v>62</v>
+      </c>
+      <c r="N17">
+        <v>2.71097507651946</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -971,8 +1273,23 @@
       <c r="I18" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18">
+        <v>18427.4017386587</v>
+      </c>
+      <c r="L18">
+        <v>210</v>
+      </c>
+      <c r="M18">
+        <v>70</v>
+      </c>
+      <c r="N18">
+        <v>3.0607783121993899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -995,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1018,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1041,7 +1358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1069,8 +1386,23 @@
       <c r="I22" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22">
+        <v>18378.890850899799</v>
+      </c>
+      <c r="L22">
+        <v>131</v>
+      </c>
+      <c r="M22">
+        <v>62</v>
+      </c>
+      <c r="N22">
+        <v>2.71097507651946</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -1098,8 +1430,23 @@
       <c r="I23" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23">
+        <v>18642.402327933502</v>
+      </c>
+      <c r="L23">
+        <v>38</v>
+      </c>
+      <c r="M23">
+        <v>55</v>
+      </c>
+      <c r="N23">
+        <v>2.4048972452995199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1127,8 +1474,23 @@
       <c r="I24" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24">
+        <v>18503.1872414916</v>
+      </c>
+      <c r="L24">
+        <v>90</v>
+      </c>
+      <c r="M24">
+        <v>55</v>
+      </c>
+      <c r="N24">
+        <v>2.4048972452995199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
@@ -1156,8 +1518,23 @@
       <c r="I25" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25">
+        <v>18406.158716150701</v>
+      </c>
+      <c r="L25">
+        <v>89</v>
+      </c>
+      <c r="M25">
+        <v>50</v>
+      </c>
+      <c r="N25">
+        <v>2.1862702229995601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>10</v>
       </c>
@@ -1183,7 +1560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17</v>
       </c>
@@ -1211,8 +1588,23 @@
       <c r="I27" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27">
+        <v>18336.618853375599</v>
+      </c>
+      <c r="L27">
+        <v>274</v>
+      </c>
+      <c r="M27">
+        <v>56</v>
+      </c>
+      <c r="N27">
+        <v>2.4486226497595101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1240,8 +1632,23 @@
       <c r="I28" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28">
+        <v>18378.190493159698</v>
+      </c>
+      <c r="L28">
+        <v>165</v>
+      </c>
+      <c r="M28">
+        <v>58</v>
+      </c>
+      <c r="N28">
+        <v>2.53607345867949</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>19</v>
       </c>
@@ -1269,8 +1676,23 @@
       <c r="I29" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K29">
+        <v>18378.239093726901</v>
+      </c>
+      <c r="L29">
+        <v>212</v>
+      </c>
+      <c r="M29">
+        <v>64</v>
+      </c>
+      <c r="N29">
+        <v>2.7984258854394399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1298,8 +1720,23 @@
       <c r="I30" s="3">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30">
+        <v>18355.601680900701</v>
+      </c>
+      <c r="L30">
+        <v>207</v>
+      </c>
+      <c r="M30">
+        <v>60</v>
+      </c>
+      <c r="N30">
+        <v>2.6235242675994801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1322,7 +1759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -1345,7 +1782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1368,7 +1805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>21</v>
       </c>
@@ -1396,8 +1833,23 @@
       <c r="I34" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34">
+        <v>18370.309753558999</v>
+      </c>
+      <c r="L34">
+        <v>167</v>
+      </c>
+      <c r="M34">
+        <v>48</v>
+      </c>
+      <c r="N34">
+        <v>2.0988194140795802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22</v>
       </c>
@@ -1425,8 +1877,23 @@
       <c r="I35" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35">
+        <v>18485.8980387501</v>
+      </c>
+      <c r="L35">
+        <v>113</v>
+      </c>
+      <c r="M35">
+        <v>54</v>
+      </c>
+      <c r="N35">
+        <v>2.3611718408395301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>23</v>
       </c>
@@ -1454,8 +1921,23 @@
       <c r="I36" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36">
+        <v>18419.1183735667</v>
+      </c>
+      <c r="L36">
+        <v>148</v>
+      </c>
+      <c r="M36">
+        <v>52</v>
+      </c>
+      <c r="N36">
+        <v>2.2737210319195502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>24</v>
       </c>
@@ -1483,8 +1965,23 @@
       <c r="I37" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>51</v>
+      </c>
+      <c r="K37">
+        <v>18396.812407933001</v>
+      </c>
+      <c r="L37">
+        <v>107</v>
+      </c>
+      <c r="M37">
+        <v>51</v>
+      </c>
+      <c r="N37">
+        <v>2.2299956274595498</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Adding more diagnostic plots
</commit_message>
<xml_diff>
--- a/models/Richards Model Parameters.xlsx
+++ b/models/Richards Model Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomo.eguchi\Documents\R\Granite_Canyon_Counts\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB28DE0-1C61-4737-9304-D744AC38E701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06DE01-A746-4829-AC6B-63FC319DD85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2745" windowWidth="19110" windowHeight="18000" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
+    <workbookView xWindow="2220" yWindow="705" windowWidth="18195" windowHeight="19395" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="50">
   <si>
     <t>K1</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Nhats</t>
   </si>
   <si>
-    <t>Horrible</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
   </si>
   <si>
     <t>v28a</t>
-  </si>
-  <si>
-    <t>Okay</t>
   </si>
 </sst>
 </file>
@@ -581,7 +572,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,19 +594,19 @@
         <v>18</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>21</v>
@@ -680,19 +671,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3">
-        <v>18456.255457203501</v>
-      </c>
-      <c r="L3">
-        <v>228</v>
-      </c>
-      <c r="M3">
-        <v>73</v>
-      </c>
-      <c r="N3">
-        <v>3.19195452557936</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -724,19 +703,7 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4">
-        <v>19096.250028757098</v>
-      </c>
-      <c r="L4">
-        <v>98</v>
-      </c>
-      <c r="M4">
-        <v>96</v>
-      </c>
-      <c r="N4">
-        <v>4.1976388281591603</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -768,19 +735,7 @@
         <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5">
-        <v>18560.823535380601</v>
-      </c>
-      <c r="L5">
-        <v>59</v>
-      </c>
-      <c r="M5">
-        <v>54</v>
-      </c>
-      <c r="N5">
-        <v>2.3611718408395301</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -812,19 +767,7 @@
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6">
-        <v>18567.872387375799</v>
-      </c>
-      <c r="L6">
-        <v>68</v>
-      </c>
-      <c r="M6">
-        <v>70</v>
-      </c>
-      <c r="N6">
-        <v>3.0607783121993899</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -931,22 +874,7 @@
         <v>5</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10">
-        <v>18377.009181113299</v>
-      </c>
-      <c r="L10">
-        <v>53</v>
-      </c>
-      <c r="M10">
-        <v>51</v>
-      </c>
-      <c r="N10">
-        <v>2.2299956274595498</v>
-      </c>
-      <c r="O10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -978,22 +906,7 @@
         <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11">
-        <v>19179.086074593601</v>
-      </c>
-      <c r="L11">
-        <v>33</v>
-      </c>
-      <c r="M11">
-        <v>82</v>
-      </c>
-      <c r="N11">
-        <v>3.5854831657192801</v>
-      </c>
-      <c r="O11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1025,22 +938,7 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12">
-        <v>18567.4568986698</v>
-      </c>
-      <c r="L12">
-        <v>44</v>
-      </c>
-      <c r="M12">
-        <v>57</v>
-      </c>
-      <c r="N12">
-        <v>2.4923480542194998</v>
-      </c>
-      <c r="O12" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1072,22 +970,7 @@
         <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13">
-        <v>18620.3893099698</v>
-      </c>
-      <c r="L13">
-        <v>49</v>
-      </c>
-      <c r="M13">
-        <v>57</v>
-      </c>
-      <c r="N13">
-        <v>2.4923480542194998</v>
-      </c>
-      <c r="O13" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1142,19 +1025,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15">
-        <v>18476.116777521998</v>
-      </c>
-      <c r="L15">
-        <v>258</v>
-      </c>
-      <c r="M15">
-        <v>68</v>
-      </c>
-      <c r="N15">
-        <v>2.97332750327941</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1186,22 +1057,10 @@
         <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16">
-        <v>18602.501768599399</v>
-      </c>
-      <c r="L16">
-        <v>76</v>
-      </c>
-      <c r="M16">
-        <v>78</v>
-      </c>
-      <c r="N16">
-        <v>3.4105815478793202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1230,22 +1089,10 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17">
-        <v>18370.9522984711</v>
-      </c>
-      <c r="L17">
-        <v>166</v>
-      </c>
-      <c r="M17">
-        <v>62</v>
-      </c>
-      <c r="N17">
-        <v>2.71097507651946</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1274,22 +1121,10 @@
         <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18">
-        <v>18427.4017386587</v>
-      </c>
-      <c r="L18">
-        <v>210</v>
-      </c>
-      <c r="M18">
-        <v>70</v>
-      </c>
-      <c r="N18">
-        <v>3.0607783121993899</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -1312,7 +1147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1335,7 +1170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +1193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1387,22 +1222,10 @@
         <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22">
-        <v>18378.890850899799</v>
-      </c>
-      <c r="L22">
-        <v>131</v>
-      </c>
-      <c r="M22">
-        <v>62</v>
-      </c>
-      <c r="N22">
-        <v>2.71097507651946</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -1431,22 +1254,10 @@
         <v>12</v>
       </c>
       <c r="J23" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23">
-        <v>18642.402327933502</v>
-      </c>
-      <c r="L23">
-        <v>38</v>
-      </c>
-      <c r="M23">
-        <v>55</v>
-      </c>
-      <c r="N23">
-        <v>2.4048972452995199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1475,22 +1286,10 @@
         <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>42</v>
-      </c>
-      <c r="K24">
-        <v>18503.1872414916</v>
-      </c>
-      <c r="L24">
-        <v>90</v>
-      </c>
-      <c r="M24">
-        <v>55</v>
-      </c>
-      <c r="N24">
-        <v>2.4048972452995199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
@@ -1519,22 +1318,10 @@
         <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>43</v>
-      </c>
-      <c r="K25">
-        <v>18406.158716150701</v>
-      </c>
-      <c r="L25">
-        <v>89</v>
-      </c>
-      <c r="M25">
-        <v>50</v>
-      </c>
-      <c r="N25">
-        <v>2.1862702229995601</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>10</v>
       </c>
@@ -1560,7 +1347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17</v>
       </c>
@@ -1589,22 +1376,10 @@
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>44</v>
-      </c>
-      <c r="K27">
-        <v>18336.618853375599</v>
-      </c>
-      <c r="L27">
-        <v>274</v>
-      </c>
-      <c r="M27">
-        <v>56</v>
-      </c>
-      <c r="N27">
-        <v>2.4486226497595101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1633,22 +1408,10 @@
         <v>11</v>
       </c>
       <c r="J28" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28">
-        <v>18378.190493159698</v>
-      </c>
-      <c r="L28">
-        <v>165</v>
-      </c>
-      <c r="M28">
-        <v>58</v>
-      </c>
-      <c r="N28">
-        <v>2.53607345867949</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>19</v>
       </c>
@@ -1677,22 +1440,10 @@
         <v>25</v>
       </c>
       <c r="J29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K29">
-        <v>18378.239093726901</v>
-      </c>
-      <c r="L29">
-        <v>212</v>
-      </c>
-      <c r="M29">
-        <v>64</v>
-      </c>
-      <c r="N29">
-        <v>2.7984258854394399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1721,22 +1472,10 @@
         <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K30">
-        <v>18355.601680900701</v>
-      </c>
-      <c r="L30">
-        <v>207</v>
-      </c>
-      <c r="M30">
-        <v>60</v>
-      </c>
-      <c r="N30">
-        <v>2.6235242675994801</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1759,7 +1498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -1805,7 +1544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>21</v>
       </c>
@@ -1834,22 +1573,10 @@
         <v>9</v>
       </c>
       <c r="J34" t="s">
-        <v>48</v>
-      </c>
-      <c r="K34">
-        <v>18370.309753558999</v>
-      </c>
-      <c r="L34">
-        <v>167</v>
-      </c>
-      <c r="M34">
-        <v>48</v>
-      </c>
-      <c r="N34">
-        <v>2.0988194140795802</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22</v>
       </c>
@@ -1878,22 +1605,10 @@
         <v>14</v>
       </c>
       <c r="J35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K35">
-        <v>18485.8980387501</v>
-      </c>
-      <c r="L35">
-        <v>113</v>
-      </c>
-      <c r="M35">
-        <v>54</v>
-      </c>
-      <c r="N35">
-        <v>2.3611718408395301</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>23</v>
       </c>
@@ -1922,22 +1637,10 @@
         <v>27</v>
       </c>
       <c r="J36" t="s">
-        <v>50</v>
-      </c>
-      <c r="K36">
-        <v>18419.1183735667</v>
-      </c>
-      <c r="L36">
-        <v>148</v>
-      </c>
-      <c r="M36">
-        <v>52</v>
-      </c>
-      <c r="N36">
-        <v>2.2737210319195502</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>24</v>
       </c>
@@ -1966,22 +1669,10 @@
         <v>28</v>
       </c>
       <c r="J37" t="s">
-        <v>51</v>
-      </c>
-      <c r="K37">
-        <v>18396.812407933001</v>
-      </c>
-      <c r="L37">
-        <v>107</v>
-      </c>
-      <c r="M37">
-        <v>51</v>
-      </c>
-      <c r="N37">
-        <v>2.2299956274595498</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Created a set of models following Gemini and Claude suggestions.
</commit_message>
<xml_diff>
--- a/models/Richards Model Parameters.xlsx
+++ b/models/Richards Model Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomo.eguchi\Documents\R\Granite_Canyon_Counts\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06DE01-A746-4829-AC6B-63FC319DD85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9903C265-C899-4BC6-9856-DB9C463EBF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="705" windowWidth="18195" windowHeight="19395" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
+    <workbookView xWindow="23895" yWindow="975" windowWidth="26325" windowHeight="20055" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Still struggling with convergence issues
</commit_message>
<xml_diff>
--- a/models/Richards Model Parameters.xlsx
+++ b/models/Richards Model Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomo.eguchi\Documents\R\Granite_Canyon_Counts\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9903C265-C899-4BC6-9856-DB9C463EBF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB3F35E-89DC-48E4-9B8D-71EFA8F50E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23895" yWindow="975" windowWidth="26325" windowHeight="20055" xr2:uid="{F6F50F0D-D1B2-41AD-AB84-EC166553B91D}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>Nhats</t>
   </si>
   <si>
-    <t>model</t>
-  </si>
-  <si>
     <t>n.big.Rhat</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>v28a</t>
+  </si>
+  <si>
+    <t>model IDs in file names</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,19 +594,19 @@
         <v>18</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>21</v>
@@ -671,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -874,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
         <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1121,7 +1121,7 @@
         <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>12</v>
       </c>
       <c r="J23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
         <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
         <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="J28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>25</v>
       </c>
       <c r="J29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>9</v>
       </c>
       <c r="J34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>14</v>
       </c>
       <c r="J35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>27</v>
       </c>
       <c r="J36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
         <v>28</v>
       </c>
       <c r="J37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>